<commit_message>
updates to plotting for common garden
</commit_message>
<xml_diff>
--- a/Planning/Inds for Planting Order CC.six.xlsx
+++ b/Planning/Inds for Planting Order CC.six.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28209"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/CatherineChamberlain/Documents/git/wildhellgarden/Planning/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="0" windowWidth="17180" windowHeight="13400" tabRatio="500"/>
+    <workbookView xWindow="2100" yWindow="520" windowWidth="17180" windowHeight="13400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,6 +19,9 @@
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -1295,6 +1303,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1620,18 +1633,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:J364"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B206" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B155" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H234" sqref="H234"/>
+      <selection pane="bottomRight" activeCell="A257" sqref="A257:XFD257"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1660,7 +1677,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1689,7 +1706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1718,7 +1735,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1747,7 +1764,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1776,7 +1793,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1805,7 +1822,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -1834,7 +1851,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1863,7 +1880,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1892,7 +1909,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1921,7 +1938,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1950,7 +1967,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1979,7 +1996,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -2008,7 +2025,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -2037,7 +2054,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -2066,7 +2083,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -2095,7 +2112,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -2124,7 +2141,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -2153,7 +2170,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -2182,7 +2199,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -2211,7 +2228,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -2240,7 +2257,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -2269,7 +2286,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -2298,7 +2315,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -2327,7 +2344,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -2356,7 +2373,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>18</v>
       </c>
@@ -2385,7 +2402,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>9</v>
       </c>
@@ -2414,7 +2431,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>20</v>
       </c>
@@ -2443,7 +2460,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -2472,7 +2489,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -2501,7 +2518,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>20</v>
       </c>
@@ -2530,7 +2547,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>14</v>
       </c>
@@ -2559,7 +2576,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>9</v>
       </c>
@@ -2588,7 +2605,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>18</v>
       </c>
@@ -2617,7 +2634,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>20</v>
       </c>
@@ -2646,7 +2663,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -2675,7 +2692,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -2704,7 +2721,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>35</v>
       </c>
@@ -2733,7 +2750,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>18</v>
       </c>
@@ -2762,7 +2779,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>14</v>
       </c>
@@ -2791,7 +2808,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>23</v>
       </c>
@@ -2820,7 +2837,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>9</v>
       </c>
@@ -2849,7 +2866,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>35</v>
       </c>
@@ -2878,7 +2895,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>35</v>
       </c>
@@ -2907,7 +2924,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>9</v>
       </c>
@@ -2936,7 +2953,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>9</v>
       </c>
@@ -2965,7 +2982,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>23</v>
       </c>
@@ -2994,7 +3011,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>20</v>
       </c>
@@ -3023,7 +3040,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>23</v>
       </c>
@@ -3052,7 +3069,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>14</v>
       </c>
@@ -3081,7 +3098,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>9</v>
       </c>
@@ -3110,7 +3127,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>35</v>
       </c>
@@ -3139,7 +3156,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>23</v>
       </c>
@@ -3168,7 +3185,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>20</v>
       </c>
@@ -3197,7 +3214,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>18</v>
       </c>
@@ -3226,7 +3243,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>20</v>
       </c>
@@ -3255,7 +3272,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>35</v>
       </c>
@@ -3284,7 +3301,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>18</v>
       </c>
@@ -3313,7 +3330,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>18</v>
       </c>
@@ -3342,7 +3359,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>18</v>
       </c>
@@ -3371,7 +3388,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>14</v>
       </c>
@@ -3400,7 +3417,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>20</v>
       </c>
@@ -3429,7 +3446,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>82</v>
       </c>
@@ -3458,7 +3475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>82</v>
       </c>
@@ -3487,7 +3504,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>86</v>
       </c>
@@ -3516,7 +3533,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>88</v>
       </c>
@@ -3545,7 +3562,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>86</v>
       </c>
@@ -3574,7 +3591,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>91</v>
       </c>
@@ -3603,7 +3620,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>91</v>
       </c>
@@ -3632,7 +3649,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>94</v>
       </c>
@@ -3661,7 +3678,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>94</v>
       </c>
@@ -3690,7 +3707,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>86</v>
       </c>
@@ -3719,7 +3736,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>88</v>
       </c>
@@ -3748,7 +3765,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>91</v>
       </c>
@@ -3777,7 +3794,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>91</v>
       </c>
@@ -3806,7 +3823,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>86</v>
       </c>
@@ -3835,7 +3852,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>94</v>
       </c>
@@ -3864,7 +3881,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>88</v>
       </c>
@@ -3893,7 +3910,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>91</v>
       </c>
@@ -3922,7 +3939,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>86</v>
       </c>
@@ -3951,7 +3968,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>88</v>
       </c>
@@ -3980,7 +3997,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>88</v>
       </c>
@@ -4009,7 +4026,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>91</v>
       </c>
@@ -4038,7 +4055,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>91</v>
       </c>
@@ -4067,7 +4084,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>86</v>
       </c>
@@ -4096,7 +4113,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="86" spans="1:10">
+    <row r="86" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>82</v>
       </c>
@@ -4125,7 +4142,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>82</v>
       </c>
@@ -4154,7 +4171,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>91</v>
       </c>
@@ -4183,7 +4200,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="89" spans="1:10">
+    <row r="89" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>94</v>
       </c>
@@ -4212,7 +4229,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="90" spans="1:10">
+    <row r="90" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>86</v>
       </c>
@@ -4241,7 +4258,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="91" spans="1:10">
+    <row r="91" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>86</v>
       </c>
@@ -4270,7 +4287,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="92" spans="1:10">
+    <row r="92" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>91</v>
       </c>
@@ -4299,7 +4316,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="93" spans="1:10">
+    <row r="93" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>86</v>
       </c>
@@ -4328,7 +4345,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="94" spans="1:10">
+    <row r="94" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>91</v>
       </c>
@@ -4357,7 +4374,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="95" spans="1:10">
+    <row r="95" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>86</v>
       </c>
@@ -4386,7 +4403,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="96" spans="1:10">
+    <row r="96" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>82</v>
       </c>
@@ -4415,7 +4432,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="97" spans="1:10">
+    <row r="97" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>82</v>
       </c>
@@ -4444,7 +4461,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="98" spans="1:10">
+    <row r="98" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>91</v>
       </c>
@@ -4473,7 +4490,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="99" spans="1:10">
+    <row r="99" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>86</v>
       </c>
@@ -4502,7 +4519,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="100" spans="1:10">
+    <row r="100" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>88</v>
       </c>
@@ -4531,7 +4548,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="101" spans="1:10">
+    <row r="101" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>91</v>
       </c>
@@ -4560,7 +4577,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="102" spans="1:10">
+    <row r="102" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>91</v>
       </c>
@@ -4589,7 +4606,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="103" spans="1:10">
+    <row r="103" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>82</v>
       </c>
@@ -4618,7 +4635,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="104" spans="1:10">
+    <row r="104" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>91</v>
       </c>
@@ -4647,7 +4664,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="105" spans="1:10">
+    <row r="105" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>86</v>
       </c>
@@ -4676,7 +4693,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="106" spans="1:10">
+    <row r="106" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>88</v>
       </c>
@@ -4705,7 +4722,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="107" spans="1:10">
+    <row r="107" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>94</v>
       </c>
@@ -4734,7 +4751,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="108" spans="1:10">
+    <row r="108" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>94</v>
       </c>
@@ -4763,7 +4780,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="109" spans="1:10">
+    <row r="109" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>86</v>
       </c>
@@ -4792,7 +4809,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="110" spans="1:10">
+    <row r="110" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>82</v>
       </c>
@@ -4818,7 +4835,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="111" spans="1:10">
+    <row r="111" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>9</v>
       </c>
@@ -4847,7 +4864,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="112" spans="1:10">
+    <row r="112" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>23</v>
       </c>
@@ -4876,7 +4893,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="113" spans="1:10">
+    <row r="113" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>23</v>
       </c>
@@ -4905,7 +4922,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="114" spans="1:10">
+    <row r="114" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>14</v>
       </c>
@@ -4934,7 +4951,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="115" spans="1:10">
+    <row r="115" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>9</v>
       </c>
@@ -4963,7 +4980,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="116" spans="1:10">
+    <row r="116" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>35</v>
       </c>
@@ -4992,7 +5009,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="117" spans="1:10">
+    <row r="117" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>18</v>
       </c>
@@ -5021,7 +5038,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="118" spans="1:10">
+    <row r="118" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>35</v>
       </c>
@@ -5050,7 +5067,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="119" spans="1:10">
+    <row r="119" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>35</v>
       </c>
@@ -5079,7 +5096,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="120" spans="1:10">
+    <row r="120" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>35</v>
       </c>
@@ -5108,7 +5125,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="121" spans="1:10">
+    <row r="121" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>18</v>
       </c>
@@ -5137,7 +5154,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="122" spans="1:10">
+    <row r="122" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>14</v>
       </c>
@@ -5166,7 +5183,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="123" spans="1:10">
+    <row r="123" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>35</v>
       </c>
@@ -5195,7 +5212,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="124" spans="1:10">
+    <row r="124" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>14</v>
       </c>
@@ -5224,7 +5241,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="125" spans="1:10">
+    <row r="125" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>9</v>
       </c>
@@ -5253,7 +5270,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="126" spans="1:10">
+    <row r="126" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>9</v>
       </c>
@@ -5282,7 +5299,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="127" spans="1:10">
+    <row r="127" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>35</v>
       </c>
@@ -5311,7 +5328,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="128" spans="1:10">
+    <row r="128" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>14</v>
       </c>
@@ -5340,7 +5357,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="129" spans="1:10">
+    <row r="129" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>9</v>
       </c>
@@ -5369,7 +5386,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="130" spans="1:10">
+    <row r="130" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>23</v>
       </c>
@@ -5398,7 +5415,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="131" spans="1:10">
+    <row r="131" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>18</v>
       </c>
@@ -5427,7 +5444,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="132" spans="1:10">
+    <row r="132" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>23</v>
       </c>
@@ -5456,7 +5473,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="133" spans="1:10">
+    <row r="133" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>20</v>
       </c>
@@ -5485,7 +5502,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="134" spans="1:10">
+    <row r="134" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>20</v>
       </c>
@@ -5514,7 +5531,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="135" spans="1:10">
+    <row r="135" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>35</v>
       </c>
@@ -5543,7 +5560,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="136" spans="1:10">
+    <row r="136" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>9</v>
       </c>
@@ -5572,7 +5589,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="137" spans="1:10">
+    <row r="137" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>20</v>
       </c>
@@ -5601,7 +5618,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="138" spans="1:10">
+    <row r="138" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>20</v>
       </c>
@@ -5630,7 +5647,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="139" spans="1:10">
+    <row r="139" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>35</v>
       </c>
@@ -5659,7 +5676,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="140" spans="1:10">
+    <row r="140" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>23</v>
       </c>
@@ -5688,7 +5705,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="141" spans="1:10">
+    <row r="141" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>9</v>
       </c>
@@ -5717,7 +5734,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="142" spans="1:10">
+    <row r="142" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>20</v>
       </c>
@@ -5746,7 +5763,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="143" spans="1:10">
+    <row r="143" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>18</v>
       </c>
@@ -5775,7 +5792,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="144" spans="1:10">
+    <row r="144" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>35</v>
       </c>
@@ -5804,7 +5821,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="145" spans="1:10">
+    <row r="145" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>23</v>
       </c>
@@ -5833,7 +5850,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="146" spans="1:10">
+    <row r="146" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>14</v>
       </c>
@@ -5862,7 +5879,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="147" spans="1:10">
+    <row r="147" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>14</v>
       </c>
@@ -5891,7 +5908,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="148" spans="1:10">
+    <row r="148" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>35</v>
       </c>
@@ -5920,7 +5937,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="149" spans="1:10">
+    <row r="149" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>9</v>
       </c>
@@ -5949,7 +5966,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="150" spans="1:10">
+    <row r="150" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>35</v>
       </c>
@@ -5978,7 +5995,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="151" spans="1:10">
+    <row r="151" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>9</v>
       </c>
@@ -6007,7 +6024,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="152" spans="1:10">
+    <row r="152" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>9</v>
       </c>
@@ -6036,7 +6053,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="153" spans="1:10">
+    <row r="153" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>20</v>
       </c>
@@ -6065,7 +6082,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="154" spans="1:10">
+    <row r="154" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>14</v>
       </c>
@@ -6091,7 +6108,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="155" spans="1:10">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>180</v>
       </c>
@@ -6120,7 +6137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:10">
+    <row r="156" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>183</v>
       </c>
@@ -6149,7 +6166,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="157" spans="1:10">
+    <row r="157" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>185</v>
       </c>
@@ -6178,7 +6195,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="158" spans="1:10">
+    <row r="158" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>185</v>
       </c>
@@ -6207,7 +6224,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="159" spans="1:10">
+    <row r="159" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>185</v>
       </c>
@@ -6236,7 +6253,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="160" spans="1:10">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>180</v>
       </c>
@@ -6265,7 +6282,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="161" spans="1:10">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>180</v>
       </c>
@@ -6294,7 +6311,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="162" spans="1:10">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>180</v>
       </c>
@@ -6323,7 +6340,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="163" spans="1:10">
+    <row r="163" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>183</v>
       </c>
@@ -6352,7 +6369,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="164" spans="1:10">
+    <row r="164" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>183</v>
       </c>
@@ -6381,7 +6398,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="165" spans="1:10">
+    <row r="165" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>183</v>
       </c>
@@ -6410,7 +6427,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="166" spans="1:10">
+    <row r="166" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>194</v>
       </c>
@@ -6439,7 +6456,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="167" spans="1:10">
+    <row r="167" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>194</v>
       </c>
@@ -6468,7 +6485,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="168" spans="1:10">
+    <row r="168" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>185</v>
       </c>
@@ -6497,7 +6514,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="169" spans="1:10">
+    <row r="169" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>183</v>
       </c>
@@ -6526,7 +6543,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="170" spans="1:10">
+    <row r="170" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>194</v>
       </c>
@@ -6555,7 +6572,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="171" spans="1:10">
+    <row r="171" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>185</v>
       </c>
@@ -6584,7 +6601,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="172" spans="1:10">
+    <row r="172" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>185</v>
       </c>
@@ -6613,7 +6630,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="173" spans="1:10">
+    <row r="173" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>185</v>
       </c>
@@ -6642,7 +6659,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="174" spans="1:10">
+    <row r="174" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>194</v>
       </c>
@@ -6671,7 +6688,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="175" spans="1:10">
+    <row r="175" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>194</v>
       </c>
@@ -6700,7 +6717,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="176" spans="1:10">
+    <row r="176" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>185</v>
       </c>
@@ -6729,7 +6746,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="177" spans="1:10">
+    <row r="177" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>194</v>
       </c>
@@ -6758,7 +6775,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="178" spans="1:10">
+    <row r="178" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>185</v>
       </c>
@@ -6787,7 +6804,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="179" spans="1:10">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>180</v>
       </c>
@@ -6816,7 +6833,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="180" spans="1:10">
+    <row r="180" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>194</v>
       </c>
@@ -6845,7 +6862,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="181" spans="1:10">
+    <row r="181" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>194</v>
       </c>
@@ -6874,7 +6891,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="182" spans="1:10">
+    <row r="182" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>194</v>
       </c>
@@ -6903,7 +6920,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="183" spans="1:10">
+    <row r="183" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>183</v>
       </c>
@@ -6932,7 +6949,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="184" spans="1:10">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>180</v>
       </c>
@@ -6961,7 +6978,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="185" spans="1:10">
+    <row r="185" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>183</v>
       </c>
@@ -6990,7 +7007,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="186" spans="1:10">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>180</v>
       </c>
@@ -7019,7 +7036,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="187" spans="1:10">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>180</v>
       </c>
@@ -7048,7 +7065,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="188" spans="1:10">
+    <row r="188" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>183</v>
       </c>
@@ -7077,7 +7094,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="189" spans="1:10">
+    <row r="189" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>183</v>
       </c>
@@ -7106,7 +7123,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="190" spans="1:10">
+    <row r="190" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>185</v>
       </c>
@@ -7135,7 +7152,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="191" spans="1:10">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>180</v>
       </c>
@@ -7164,7 +7181,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="192" spans="1:10">
+    <row r="192" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>82</v>
       </c>
@@ -7193,7 +7210,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="193" spans="1:10">
+    <row r="193" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>88</v>
       </c>
@@ -7222,7 +7239,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="194" spans="1:10">
+    <row r="194" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>88</v>
       </c>
@@ -7251,7 +7268,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="195" spans="1:10">
+    <row r="195" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>94</v>
       </c>
@@ -7280,7 +7297,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="196" spans="1:10">
+    <row r="196" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>91</v>
       </c>
@@ -7309,7 +7326,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="197" spans="1:10">
+    <row r="197" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>82</v>
       </c>
@@ -7338,7 +7355,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="198" spans="1:10">
+    <row r="198" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>91</v>
       </c>
@@ -7367,7 +7384,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="199" spans="1:10">
+    <row r="199" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>82</v>
       </c>
@@ -7396,7 +7413,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="200" spans="1:10">
+    <row r="200" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>91</v>
       </c>
@@ -7425,7 +7442,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="201" spans="1:10">
+    <row r="201" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>82</v>
       </c>
@@ -7454,7 +7471,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="202" spans="1:10">
+    <row r="202" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>94</v>
       </c>
@@ -7483,7 +7500,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="203" spans="1:10">
+    <row r="203" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>94</v>
       </c>
@@ -7512,7 +7529,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="204" spans="1:10">
+    <row r="204" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>86</v>
       </c>
@@ -7541,7 +7558,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="205" spans="1:10">
+    <row r="205" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>82</v>
       </c>
@@ -7570,7 +7587,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="206" spans="1:10">
+    <row r="206" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>94</v>
       </c>
@@ -7599,7 +7616,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="207" spans="1:10">
+    <row r="207" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>94</v>
       </c>
@@ -7628,7 +7645,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="208" spans="1:10">
+    <row r="208" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>88</v>
       </c>
@@ -7657,7 +7674,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="209" spans="1:10">
+    <row r="209" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>88</v>
       </c>
@@ -7686,7 +7703,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="210" spans="1:10">
+    <row r="210" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>86</v>
       </c>
@@ -7715,7 +7732,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="211" spans="1:10">
+    <row r="211" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>82</v>
       </c>
@@ -7744,7 +7761,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="212" spans="1:10">
+    <row r="212" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>91</v>
       </c>
@@ -7773,7 +7790,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="213" spans="1:10">
+    <row r="213" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>88</v>
       </c>
@@ -7802,7 +7819,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="214" spans="1:10">
+    <row r="214" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>88</v>
       </c>
@@ -7831,7 +7848,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="215" spans="1:10">
+    <row r="215" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>86</v>
       </c>
@@ -7860,7 +7877,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="216" spans="1:10">
+    <row r="216" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>94</v>
       </c>
@@ -7889,7 +7906,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="217" spans="1:10">
+    <row r="217" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>94</v>
       </c>
@@ -7918,7 +7935,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="218" spans="1:10">
+    <row r="218" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>94</v>
       </c>
@@ -7947,7 +7964,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="219" spans="1:10">
+    <row r="219" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>86</v>
       </c>
@@ -7976,7 +7993,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="220" spans="1:10">
+    <row r="220" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>86</v>
       </c>
@@ -8005,7 +8022,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="221" spans="1:10">
+    <row r="221" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>91</v>
       </c>
@@ -8034,7 +8051,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="222" spans="1:10">
+    <row r="222" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>82</v>
       </c>
@@ -8063,7 +8080,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="223" spans="1:10">
+    <row r="223" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>94</v>
       </c>
@@ -8092,7 +8109,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="224" spans="1:10">
+    <row r="224" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>88</v>
       </c>
@@ -8121,7 +8138,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="225" spans="1:10">
+    <row r="225" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>86</v>
       </c>
@@ -8150,7 +8167,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="226" spans="1:10">
+    <row r="226" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>86</v>
       </c>
@@ -8179,7 +8196,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="227" spans="1:10">
+    <row r="227" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>82</v>
       </c>
@@ -8208,7 +8225,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="228" spans="1:10">
+    <row r="228" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>82</v>
       </c>
@@ -8237,7 +8254,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="229" spans="1:10">
+    <row r="229" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>88</v>
       </c>
@@ -8266,7 +8283,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="230" spans="1:10">
+    <row r="230" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>82</v>
       </c>
@@ -8295,7 +8312,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="231" spans="1:10">
+    <row r="231" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>94</v>
       </c>
@@ -8324,7 +8341,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="232" spans="1:10">
+    <row r="232" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>82</v>
       </c>
@@ -8353,7 +8370,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="233" spans="1:10">
+    <row r="233" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>86</v>
       </c>
@@ -8382,7 +8399,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="234" spans="1:10">
+    <row r="234" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>86</v>
       </c>
@@ -8411,7 +8428,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="235" spans="1:10">
+    <row r="235" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>91</v>
       </c>
@@ -8440,7 +8457,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="236" spans="1:10">
+    <row r="236" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>91</v>
       </c>
@@ -8469,7 +8486,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="237" spans="1:10">
+    <row r="237" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>94</v>
       </c>
@@ -8498,7 +8515,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="238" spans="1:10">
+    <row r="238" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>18</v>
       </c>
@@ -8527,7 +8544,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="239" spans="1:10">
+    <row r="239" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>23</v>
       </c>
@@ -8556,7 +8573,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="240" spans="1:10">
+    <row r="240" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>23</v>
       </c>
@@ -8585,7 +8602,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="241" spans="1:10">
+    <row r="241" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>23</v>
       </c>
@@ -8614,7 +8631,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="242" spans="1:10">
+    <row r="242" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>23</v>
       </c>
@@ -8643,7 +8660,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="243" spans="1:10">
+    <row r="243" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>14</v>
       </c>
@@ -8672,7 +8689,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="244" spans="1:10">
+    <row r="244" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>9</v>
       </c>
@@ -8701,7 +8718,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="245" spans="1:10">
+    <row r="245" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>18</v>
       </c>
@@ -8730,7 +8747,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="246" spans="1:10">
+    <row r="246" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>23</v>
       </c>
@@ -8759,7 +8776,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="247" spans="1:10">
+    <row r="247" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>14</v>
       </c>
@@ -8788,7 +8805,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="248" spans="1:10">
+    <row r="248" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>20</v>
       </c>
@@ -8817,7 +8834,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="249" spans="1:10">
+    <row r="249" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>23</v>
       </c>
@@ -8846,7 +8863,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="250" spans="1:10">
+    <row r="250" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>14</v>
       </c>
@@ -8872,7 +8889,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="251" spans="1:10">
+    <row r="251" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>20</v>
       </c>
@@ -8901,7 +8918,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="252" spans="1:10">
+    <row r="252" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>185</v>
       </c>
@@ -8930,7 +8947,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="253" spans="1:10">
+    <row r="253" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>183</v>
       </c>
@@ -8959,7 +8976,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="254" spans="1:10">
+    <row r="254" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>180</v>
       </c>
@@ -8988,7 +9005,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="255" spans="1:10">
+    <row r="255" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>180</v>
       </c>
@@ -9017,7 +9034,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="256" spans="1:10">
+    <row r="256" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>180</v>
       </c>
@@ -9046,7 +9063,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="257" spans="1:10">
+    <row r="257" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>183</v>
       </c>
@@ -9075,7 +9092,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="258" spans="1:10">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>180</v>
       </c>
@@ -9104,7 +9121,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="259" spans="1:10">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>180</v>
       </c>
@@ -9133,7 +9150,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="260" spans="1:10">
+    <row r="260" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>183</v>
       </c>
@@ -9162,7 +9179,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="261" spans="1:10">
+    <row r="261" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>183</v>
       </c>
@@ -9191,7 +9208,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="262" spans="1:10">
+    <row r="262" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>183</v>
       </c>
@@ -9220,7 +9237,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="263" spans="1:10">
+    <row r="263" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>185</v>
       </c>
@@ -9249,7 +9266,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="264" spans="1:10">
+    <row r="264" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>194</v>
       </c>
@@ -9278,7 +9295,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="265" spans="1:10">
+    <row r="265" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>194</v>
       </c>
@@ -9307,7 +9324,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="266" spans="1:10">
+    <row r="266" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>194</v>
       </c>
@@ -9336,7 +9353,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="267" spans="1:10">
+    <row r="267" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>183</v>
       </c>
@@ -9365,7 +9382,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="268" spans="1:10">
+    <row r="268" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>185</v>
       </c>
@@ -9394,7 +9411,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="269" spans="1:10">
+    <row r="269" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>180</v>
       </c>
@@ -9423,7 +9440,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="270" spans="1:10">
+    <row r="270" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>194</v>
       </c>
@@ -9452,7 +9469,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="271" spans="1:10">
+    <row r="271" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>185</v>
       </c>
@@ -9481,7 +9498,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="272" spans="1:10">
+    <row r="272" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>185</v>
       </c>
@@ -9510,7 +9527,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="273" spans="1:10">
+    <row r="273" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>180</v>
       </c>
@@ -9539,7 +9556,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="274" spans="1:10">
+    <row r="274" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>183</v>
       </c>
@@ -9568,7 +9585,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="275" spans="1:10">
+    <row r="275" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>183</v>
       </c>
@@ -9597,7 +9614,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="276" spans="1:10">
+    <row r="276" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>185</v>
       </c>
@@ -9626,7 +9643,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="277" spans="1:10">
+    <row r="277" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>194</v>
       </c>
@@ -9655,7 +9672,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="278" spans="1:10">
+    <row r="278" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>180</v>
       </c>
@@ -9684,7 +9701,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="279" spans="1:10">
+    <row r="279" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>185</v>
       </c>
@@ -9713,7 +9730,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="280" spans="1:10">
+    <row r="280" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>194</v>
       </c>
@@ -9742,7 +9759,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="281" spans="1:10">
+    <row r="281" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>180</v>
       </c>
@@ -9771,7 +9788,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="282" spans="1:10">
+    <row r="282" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>183</v>
       </c>
@@ -9800,7 +9817,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="283" spans="1:10">
+    <row r="283" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>194</v>
       </c>
@@ -9829,7 +9846,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="284" spans="1:10">
+    <row r="284" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>194</v>
       </c>
@@ -9858,7 +9875,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="285" spans="1:10">
+    <row r="285" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>185</v>
       </c>
@@ -9887,7 +9904,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="286" spans="1:10">
+    <row r="286" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>185</v>
       </c>
@@ -9916,7 +9933,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="287" spans="1:10">
+    <row r="287" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>194</v>
       </c>
@@ -9945,7 +9962,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="288" spans="1:10">
+    <row r="288" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>180</v>
       </c>
@@ -9974,7 +9991,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="289" spans="1:10">
+    <row r="289" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>88</v>
       </c>
@@ -10003,7 +10020,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="290" spans="1:10">
+    <row r="290" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>91</v>
       </c>
@@ -10032,7 +10049,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="291" spans="1:10">
+    <row r="291" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>88</v>
       </c>
@@ -10061,7 +10078,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="292" spans="1:10">
+    <row r="292" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>86</v>
       </c>
@@ -10090,7 +10107,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="293" spans="1:10">
+    <row r="293" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>82</v>
       </c>
@@ -10119,7 +10136,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="294" spans="1:10">
+    <row r="294" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>94</v>
       </c>
@@ -10148,7 +10165,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="295" spans="1:10">
+    <row r="295" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>91</v>
       </c>
@@ -10177,7 +10194,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="296" spans="1:10">
+    <row r="296" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>88</v>
       </c>
@@ -10206,7 +10223,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="297" spans="1:10">
+    <row r="297" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>94</v>
       </c>
@@ -10235,7 +10252,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="298" spans="1:10">
+    <row r="298" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>91</v>
       </c>
@@ -10264,7 +10281,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="299" spans="1:10">
+    <row r="299" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>94</v>
       </c>
@@ -10293,7 +10310,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="300" spans="1:10">
+    <row r="300" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>88</v>
       </c>
@@ -10322,7 +10339,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="301" spans="1:10">
+    <row r="301" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>86</v>
       </c>
@@ -10351,7 +10368,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="302" spans="1:10">
+    <row r="302" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
         <v>82</v>
       </c>
@@ -10380,7 +10397,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="303" spans="1:10">
+    <row r="303" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>88</v>
       </c>
@@ -10409,7 +10426,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="304" spans="1:10">
+    <row r="304" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
         <v>82</v>
       </c>
@@ -10438,7 +10455,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="305" spans="1:10">
+    <row r="305" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>94</v>
       </c>
@@ -10467,7 +10484,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="306" spans="1:10">
+    <row r="306" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>94</v>
       </c>
@@ -10496,7 +10513,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="307" spans="1:10">
+    <row r="307" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
         <v>82</v>
       </c>
@@ -10525,7 +10542,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="308" spans="1:10">
+    <row r="308" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
         <v>88</v>
       </c>
@@ -10554,7 +10571,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="309" spans="1:10">
+    <row r="309" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
         <v>88</v>
       </c>
@@ -10583,7 +10600,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="310" spans="1:10">
+    <row r="310" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
         <v>94</v>
       </c>
@@ -10612,7 +10629,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="311" spans="1:10">
+    <row r="311" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
         <v>88</v>
       </c>
@@ -10641,7 +10658,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="312" spans="1:10">
+    <row r="312" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
         <v>94</v>
       </c>
@@ -10670,7 +10687,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="313" spans="1:10">
+    <row r="313" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
         <v>82</v>
       </c>
@@ -10699,7 +10716,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="314" spans="1:10">
+    <row r="314" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
         <v>88</v>
       </c>
@@ -10728,7 +10745,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="315" spans="1:10">
+    <row r="315" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
         <v>18</v>
       </c>
@@ -10757,7 +10774,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="316" spans="1:10">
+    <row r="316" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
         <v>14</v>
       </c>
@@ -10786,7 +10803,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="317" spans="1:10">
+    <row r="317" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
         <v>14</v>
       </c>
@@ -10815,7 +10832,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="318" spans="1:10">
+    <row r="318" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
         <v>14</v>
       </c>
@@ -10844,7 +10861,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="319" spans="1:10">
+    <row r="319" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
         <v>9</v>
       </c>
@@ -10873,7 +10890,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="320" spans="1:10">
+    <row r="320" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
         <v>20</v>
       </c>
@@ -10902,7 +10919,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="321" spans="1:10">
+    <row r="321" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
         <v>18</v>
       </c>
@@ -10931,7 +10948,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="322" spans="1:10">
+    <row r="322" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
         <v>20</v>
       </c>
@@ -10960,7 +10977,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="323" spans="1:10">
+    <row r="323" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
         <v>23</v>
       </c>
@@ -10989,7 +11006,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="324" spans="1:10">
+    <row r="324" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
         <v>23</v>
       </c>
@@ -11018,7 +11035,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="325" spans="1:10">
+    <row r="325" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
         <v>9</v>
       </c>
@@ -11047,7 +11064,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="326" spans="1:10">
+    <row r="326" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
         <v>20</v>
       </c>
@@ -11076,7 +11093,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="327" spans="1:10">
+    <row r="327" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
         <v>35</v>
       </c>
@@ -11105,7 +11122,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="328" spans="1:10">
+    <row r="328" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
         <v>180</v>
       </c>
@@ -11134,7 +11151,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="329" spans="1:10">
+    <row r="329" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
         <v>183</v>
       </c>
@@ -11163,7 +11180,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="330" spans="1:10">
+    <row r="330" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
         <v>185</v>
       </c>
@@ -11192,7 +11209,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="331" spans="1:10">
+    <row r="331" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
         <v>183</v>
       </c>
@@ -11221,7 +11238,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="332" spans="1:10">
+    <row r="332" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
         <v>194</v>
       </c>
@@ -11250,7 +11267,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="333" spans="1:10">
+    <row r="333" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
         <v>183</v>
       </c>
@@ -11279,7 +11296,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="334" spans="1:10">
+    <row r="334" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
         <v>185</v>
       </c>
@@ -11308,7 +11325,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="335" spans="1:10">
+    <row r="335" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A335" t="s">
         <v>185</v>
       </c>
@@ -11337,7 +11354,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="336" spans="1:10">
+    <row r="336" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
         <v>194</v>
       </c>
@@ -11366,7 +11383,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="337" spans="1:10">
+    <row r="337" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
         <v>183</v>
       </c>
@@ -11395,7 +11412,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="338" spans="1:10">
+    <row r="338" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A338" t="s">
         <v>180</v>
       </c>
@@ -11424,7 +11441,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="339" spans="1:10">
+    <row r="339" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A339" t="s">
         <v>194</v>
       </c>
@@ -11453,7 +11470,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="340" spans="1:10">
+    <row r="340" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A340" t="s">
         <v>194</v>
       </c>
@@ -11482,7 +11499,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="341" spans="1:10">
+    <row r="341" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A341" t="s">
         <v>183</v>
       </c>
@@ -11511,7 +11528,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="342" spans="1:10">
+    <row r="342" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A342" t="s">
         <v>185</v>
       </c>
@@ -11540,7 +11557,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="343" spans="1:10">
+    <row r="343" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A343" t="s">
         <v>194</v>
       </c>
@@ -11569,7 +11586,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="344" spans="1:10">
+    <row r="344" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A344" t="s">
         <v>283</v>
       </c>
@@ -11598,7 +11615,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="345" spans="1:10">
+    <row r="345" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A345" t="s">
         <v>183</v>
       </c>
@@ -11627,7 +11644,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="346" spans="1:10">
+    <row r="346" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A346" t="s">
         <v>185</v>
       </c>
@@ -11656,7 +11673,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="347" spans="1:10">
+    <row r="347" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A347" t="s">
         <v>180</v>
       </c>
@@ -11685,7 +11702,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="348" spans="1:10">
+    <row r="348" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
         <v>180</v>
       </c>
@@ -11714,7 +11731,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="349" spans="1:10">
+    <row r="349" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A349" t="s">
         <v>194</v>
       </c>
@@ -11743,7 +11760,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="350" spans="1:10">
+    <row r="350" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A350" t="s">
         <v>183</v>
       </c>
@@ -11772,7 +11789,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="351" spans="1:10">
+    <row r="351" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A351" t="s">
         <v>183</v>
       </c>
@@ -11801,7 +11818,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="352" spans="1:10">
+    <row r="352" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A352" t="s">
         <v>183</v>
       </c>
@@ -11830,7 +11847,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="353" spans="1:10">
+    <row r="353" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A353" t="s">
         <v>23</v>
       </c>
@@ -11859,7 +11876,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="354" spans="1:10">
+    <row r="354" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A354" t="s">
         <v>18</v>
       </c>
@@ -11888,7 +11905,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="355" spans="1:10">
+    <row r="355" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A355" t="s">
         <v>20</v>
       </c>
@@ -11917,7 +11934,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="356" spans="1:10">
+    <row r="356" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A356" t="s">
         <v>23</v>
       </c>
@@ -11946,7 +11963,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="357" spans="1:10">
+    <row r="357" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A357" t="s">
         <v>35</v>
       </c>
@@ -11975,7 +11992,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="358" spans="1:10">
+    <row r="358" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A358" t="s">
         <v>35</v>
       </c>
@@ -12004,7 +12021,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="359" spans="1:10">
+    <row r="359" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A359" t="s">
         <v>14</v>
       </c>
@@ -12033,7 +12050,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="360" spans="1:10">
+    <row r="360" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A360" t="s">
         <v>14</v>
       </c>
@@ -12062,7 +12079,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="361" spans="1:10">
+    <row r="361" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A361" t="s">
         <v>14</v>
       </c>
@@ -12091,7 +12108,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="362" spans="1:10">
+    <row r="362" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A362" t="s">
         <v>18</v>
       </c>
@@ -12120,7 +12137,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="363" spans="1:10">
+    <row r="363" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A363" t="s">
         <v>20</v>
       </c>
@@ -12149,7 +12166,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="364" spans="1:10">
+    <row r="364" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A364" t="s">
         <v>20</v>
       </c>
@@ -12179,14 +12196,15 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F364"/>
+  <autoFilter ref="A1:F364">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="0.75"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>